<commit_message>
rename db to db_proxy
</commit_message>
<xml_diff>
--- a/resource/excel/squick/DB.xlsx
+++ b/resource/excel/squick/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26136" windowHeight="16260"/>
+    <workbookView windowWidth="22920" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="property" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Id</t>
   </si>
@@ -70,13 +70,16 @@
     <t>RedisServer_1</t>
   </si>
   <si>
-    <t>001</t>
+    <t>1</t>
   </si>
   <si>
     <t>1.14.123.62</t>
   </si>
   <si>
-    <t>indieleague</t>
+    <t>pwnsky_squick</t>
+  </si>
+  <si>
+    <t>MysqlServer_1</t>
   </si>
 </sst>
 </file>
@@ -839,7 +842,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -886,9 +889,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1216,17 +1216,17 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="24.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="19.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="19.5583333333333" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="33.6666666666667" customWidth="1"/>
-    <col min="5" max="5" width="24.5555555555556" customWidth="1"/>
-    <col min="6" max="6" width="32.5555555555556" customWidth="1"/>
+    <col min="5" max="5" width="24.5583333333333" customWidth="1"/>
+    <col min="6" max="6" width="32.5583333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" ht="15.15" spans="1:6">
+    <row r="10" ht="14.25" spans="1:6">
       <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
@@ -1435,17 +1435,29 @@
       <c r="E11" s="16">
         <v>22222</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="A12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="16">
+        <v>2</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="16">
+        <v>10086</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>